<commit_message>
Add all stats to Tank Upgrade
</commit_message>
<xml_diff>
--- a/Documentation/Balance/Balance.xlsx
+++ b/Documentation/Balance/Balance.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Tank-Survivors\Documentation\Balance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0070B725-2C19-46AE-84FE-DE76770BE505}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A66753B5-A212-4A67-ACC9-4D856E751177}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-11352" yWindow="1740" windowWidth="23040" windowHeight="13644" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-15648" yWindow="4968" windowWidth="23040" windowHeight="13644" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -790,8 +790,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AG98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1326,7 +1326,7 @@
       <c r="X11" s="1"/>
       <c r="Y11" s="1"/>
       <c r="Z11" s="18">
-        <f t="shared" ref="Z11:Z21" si="1">SUM(D11:J11,L11:P11,R11:Y11)</f>
+        <f t="shared" ref="Z11:Z14" si="1">SUM(D11:J11,L11:P11,R11:Y11)</f>
         <v>0.3</v>
       </c>
       <c r="AA11" s="1" t="s">
@@ -1838,7 +1838,7 @@
       <c r="X22" s="1"/>
       <c r="Y22" s="1"/>
       <c r="Z22" s="18">
-        <f>SUM(D22:J22,L22:P22,R22:Y22)</f>
+        <f t="shared" ref="Z22:Z28" si="2">SUM(D22:J22,L22:P22,R22:Y22)</f>
         <v>14</v>
       </c>
       <c r="AA22" s="1" t="s">
@@ -1883,7 +1883,7 @@
       <c r="X23" s="1"/>
       <c r="Y23" s="1"/>
       <c r="Z23" s="18">
-        <f>SUM(D23:J23,L23:P23,R23:Y23)</f>
+        <f t="shared" si="2"/>
         <v>0.15000000000000002</v>
       </c>
       <c r="AA23" s="1" t="s">
@@ -1938,7 +1938,7 @@
       <c r="X24" s="1"/>
       <c r="Y24" s="1"/>
       <c r="Z24" s="18">
-        <f>SUM(D24:J24,L24:P24,R24:Y24)</f>
+        <f t="shared" si="2"/>
         <v>120</v>
       </c>
       <c r="AA24" s="1" t="s">
@@ -1989,7 +1989,7 @@
       </c>
       <c r="Y25" s="1"/>
       <c r="Z25" s="18">
-        <f>SUM(D25:J25,L25:P25,R25:Y25)</f>
+        <f t="shared" si="2"/>
         <v>230</v>
       </c>
       <c r="AA25" s="1" t="s">
@@ -2046,7 +2046,7 @@
       <c r="X26" s="1"/>
       <c r="Y26" s="1"/>
       <c r="Z26" s="18">
-        <f>SUM(D26:J26,L26:P26,R26:Y26)</f>
+        <f t="shared" si="2"/>
         <v>14</v>
       </c>
       <c r="AA26" s="1" t="s">
@@ -2099,7 +2099,7 @@
       <c r="X27" s="1"/>
       <c r="Y27" s="1"/>
       <c r="Z27" s="18">
-        <f>SUM(D27:J27,L27:P27,R27:Y27)</f>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="AA27" s="1" t="s">
@@ -2148,7 +2148,7 @@
       </c>
       <c r="Y28" s="1"/>
       <c r="Z28" s="18">
-        <f>SUM(D28:J28,L28:P28,R28:Y28)</f>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="AA28" s="1" t="s">
@@ -2414,7 +2414,7 @@
       <c r="X34" s="1"/>
       <c r="Y34" s="1"/>
       <c r="Z34" s="18">
-        <f t="shared" ref="Z34:Z37" si="2">SUM(D34:J34,L34:P34,R34:Y34)</f>
+        <f t="shared" ref="Z34:Z36" si="3">SUM(D34:J34,L34:P34,R34:Y34)</f>
         <v>1.4000000000000001</v>
       </c>
       <c r="AA34" s="1" t="s">
@@ -2459,7 +2459,7 @@
       <c r="X35" s="1"/>
       <c r="Y35" s="1"/>
       <c r="Z35" s="18">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>20</v>
       </c>
       <c r="AA35" s="1" t="s">
@@ -2502,7 +2502,7 @@
       <c r="X36" s="1"/>
       <c r="Y36" s="1"/>
       <c r="Z36" s="18">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>100</v>
       </c>
       <c r="AA36" s="1" t="s">
@@ -2549,7 +2549,7 @@
       <c r="X37" s="1"/>
       <c r="Y37" s="1"/>
       <c r="Z37" s="18">
-        <f>SUM(D37:J37,L37:P37,R37:Y37)</f>
+        <f t="shared" ref="Z37:Z50" si="4">SUM(D37:J37,L37:P37,R37:Y37)</f>
         <v>7</v>
       </c>
       <c r="AA37" s="1" t="s">
@@ -2596,7 +2596,7 @@
       <c r="X38" s="1"/>
       <c r="Y38" s="1"/>
       <c r="Z38" s="18">
-        <f>SUM(D38:J38,L38:P38,R38:Y38)</f>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
       <c r="AA38" s="1" t="s">
@@ -2643,7 +2643,7 @@
       <c r="X39" s="1"/>
       <c r="Y39" s="1"/>
       <c r="Z39" s="18">
-        <f>SUM(D39:J39,L39:P39,R39:Y39)</f>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="AA39" s="1" t="s">
@@ -2690,7 +2690,7 @@
       <c r="X40" s="1"/>
       <c r="Y40" s="1"/>
       <c r="Z40" s="18">
-        <f>SUM(D40:J40,L40:P40,R40:Y40)</f>
+        <f t="shared" si="4"/>
         <v>25</v>
       </c>
       <c r="AA40" s="1" t="s">
@@ -2737,7 +2737,7 @@
       <c r="X41" s="1"/>
       <c r="Y41" s="1"/>
       <c r="Z41" s="18">
-        <f>SUM(D41:J41,L41:P41,R41:Y41)</f>
+        <f t="shared" si="4"/>
         <v>20</v>
       </c>
       <c r="AA41" s="1" t="s">
@@ -2786,7 +2786,7 @@
       <c r="X42" s="25"/>
       <c r="Y42" s="25"/>
       <c r="Z42" s="27">
-        <f>SUM(D42:J42,L42:P42,R42:Y42)</f>
+        <f t="shared" si="4"/>
         <v>35</v>
       </c>
       <c r="AA42" s="25" t="s">
@@ -2835,7 +2835,7 @@
       <c r="X43" s="25"/>
       <c r="Y43" s="25"/>
       <c r="Z43" s="27">
-        <f>SUM(D43:J43,L43:P43,R43:Y43)</f>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="AA43" s="25" t="s">
@@ -2880,7 +2880,7 @@
       <c r="X44" s="25"/>
       <c r="Y44" s="25"/>
       <c r="Z44" s="27">
-        <f>SUM(D44:J44,L44:P44,R44:Y44)</f>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="AA44" s="25" t="s">
@@ -2927,7 +2927,7 @@
       <c r="X45" s="25"/>
       <c r="Y45" s="25"/>
       <c r="Z45" s="27">
-        <f>SUM(D45:J45,L45:P45,R45:Y45)</f>
+        <f t="shared" si="4"/>
         <v>5</v>
       </c>
       <c r="AA45" s="25" t="s">
@@ -2972,7 +2972,7 @@
       <c r="X46" s="25"/>
       <c r="Y46" s="25"/>
       <c r="Z46" s="27">
-        <f>SUM(D46:J46,L46:P46,R46:Y46)</f>
+        <f t="shared" si="4"/>
         <v>0.3</v>
       </c>
       <c r="AA46" s="25" t="s">
@@ -3023,7 +3023,7 @@
       </c>
       <c r="Y47" s="25"/>
       <c r="Z47" s="27">
-        <f>SUM(D47:J47,L47:P47,R47:Y47)</f>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
       <c r="AA47" s="25" t="s">
@@ -3074,7 +3074,7 @@
       </c>
       <c r="Y48" s="1"/>
       <c r="Z48" s="18">
-        <f>SUM(D48:J48,L48:P48,R48:Y48)</f>
+        <f t="shared" si="4"/>
         <v>25</v>
       </c>
       <c r="AA48" s="1" t="s">
@@ -3125,7 +3125,7 @@
         <v>-0.02</v>
       </c>
       <c r="Z49" s="18">
-        <f>SUM(D49:J49,L49:P49,R49:Y49)</f>
+        <f t="shared" si="4"/>
         <v>5.0000000000000017E-2</v>
       </c>
       <c r="AA49" s="1" t="s">
@@ -3176,7 +3176,7 @@
       </c>
       <c r="Y50" s="8"/>
       <c r="Z50" s="18">
-        <f>SUM(D50:J50,L50:P50,R50:Y50)</f>
+        <f t="shared" si="4"/>
         <v>6</v>
       </c>
       <c r="AA50" s="8" t="s">
@@ -3378,7 +3378,7 @@
       <c r="X54" s="1"/>
       <c r="Y54" s="1"/>
       <c r="Z54" s="18">
-        <f t="shared" ref="Z54:Z63" si="3">SUM(D54:J54,L54:P54,R54:Y54)</f>
+        <f t="shared" ref="Z54:Z63" si="5">SUM(D54:J54,L54:P54,R54:Y54)</f>
         <v>4.7</v>
       </c>
       <c r="AA54" s="1" t="s">
@@ -3427,7 +3427,7 @@
       <c r="X55" s="1"/>
       <c r="Y55" s="1"/>
       <c r="Z55" s="18">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>100</v>
       </c>
       <c r="AA55" s="1" t="s">
@@ -3476,7 +3476,7 @@
       <c r="X56" s="1"/>
       <c r="Y56" s="1"/>
       <c r="Z56" s="18">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>200</v>
       </c>
       <c r="AA56" s="1" t="s">
@@ -3525,7 +3525,7 @@
       <c r="X57" s="1"/>
       <c r="Y57" s="1"/>
       <c r="Z57" s="18">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>20</v>
       </c>
       <c r="AA57" s="1" t="s">
@@ -3566,7 +3566,7 @@
       <c r="X58" s="1"/>
       <c r="Y58" s="1"/>
       <c r="Z58" s="18">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AA58" s="1" t="s">
@@ -3617,7 +3617,7 @@
       <c r="X59" s="1"/>
       <c r="Y59" s="1"/>
       <c r="Z59" s="18">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>4.5</v>
       </c>
       <c r="AA59" s="1" t="s">
@@ -3664,7 +3664,7 @@
       </c>
       <c r="Y60" s="1"/>
       <c r="Z60" s="18">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>25</v>
       </c>
       <c r="AA60" s="1" t="s">
@@ -3709,7 +3709,7 @@
       <c r="X61" s="1"/>
       <c r="Y61" s="1"/>
       <c r="Z61" s="18">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>2</v>
       </c>
       <c r="AA61" s="1" t="s">
@@ -3766,7 +3766,7 @@
       <c r="X62" s="1"/>
       <c r="Y62" s="1"/>
       <c r="Z62" s="18">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>5.000000000000001E-2</v>
       </c>
       <c r="AA62" s="1" t="s">
@@ -3809,7 +3809,7 @@
       <c r="X63" s="8"/>
       <c r="Y63" s="8"/>
       <c r="Z63" s="19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>100</v>
       </c>
       <c r="AA63" s="8" t="s">

</xml_diff>

<commit_message>
Add stats for double gun
</commit_message>
<xml_diff>
--- a/Documentation/Balance/Balance.xlsx
+++ b/Documentation/Balance/Balance.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Tank-Survivors\Documentation\Balance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5B4DD31-C40F-451B-AB97-765467B739B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C99EC3AD-0CDD-49A8-BA17-3774B8EB51F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3744" yWindow="16020" windowWidth="23040" windowHeight="13644" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3744" yWindow="4956" windowWidth="23040" windowHeight="13644" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -796,8 +796,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AG98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="T12" sqref="T12"/>
+    <sheetView tabSelected="1" topLeftCell="O1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="V9" sqref="V9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1378,13 +1378,17 @@
       <c r="S12" s="1"/>
       <c r="T12" s="1"/>
       <c r="U12" s="1"/>
-      <c r="V12" s="1"/>
+      <c r="V12" s="1">
+        <v>15</v>
+      </c>
       <c r="W12" s="1"/>
       <c r="X12" s="1"/>
-      <c r="Y12" s="1"/>
+      <c r="Y12" s="1">
+        <v>20</v>
+      </c>
       <c r="Z12" s="18">
         <f>SUM(D12:J12,L12:P12,R12:Y12)</f>
-        <v>35</v>
+        <v>70</v>
       </c>
       <c r="AA12" s="1" t="s">
         <v>6</v>
@@ -1475,15 +1479,13 @@
       <c r="S14" s="1"/>
       <c r="T14" s="1"/>
       <c r="U14" s="1"/>
-      <c r="V14" s="1">
-        <v>4</v>
-      </c>
+      <c r="V14" s="1"/>
       <c r="W14" s="1"/>
       <c r="X14" s="1"/>
       <c r="Y14" s="1"/>
       <c r="Z14" s="18">
         <f t="shared" si="1"/>
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="AA14" s="1" t="s">
         <v>26</v>
@@ -1570,18 +1572,20 @@
         <v>90</v>
       </c>
       <c r="R16" s="1"/>
-      <c r="S16" s="1"/>
+      <c r="S16" s="1">
+        <v>1</v>
+      </c>
       <c r="T16" s="1"/>
       <c r="U16" s="1"/>
       <c r="V16" s="1"/>
       <c r="W16" s="1"/>
       <c r="X16" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="Y16" s="1"/>
       <c r="Z16" s="18">
         <f>SUM(D16:J16,L16:P16,R16:Y16)</f>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="AA16" s="1" t="s">
         <v>29</v>
@@ -1623,12 +1627,14 @@
       <c r="T17" s="1"/>
       <c r="U17" s="1"/>
       <c r="V17" s="1"/>
-      <c r="W17" s="1"/>
+      <c r="W17" s="1">
+        <v>10</v>
+      </c>
       <c r="X17" s="1"/>
       <c r="Y17" s="1"/>
       <c r="Z17" s="18">
         <f>SUM(D17:J17,L17:P17,R17:Y17)</f>
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="AA17" s="1" t="s">
         <v>30</v>
@@ -1716,7 +1722,9 @@
       <c r="T19" s="8"/>
       <c r="U19" s="8"/>
       <c r="V19" s="8"/>
-      <c r="W19" s="8"/>
+      <c r="W19" s="8">
+        <v>5</v>
+      </c>
       <c r="X19" s="8"/>
       <c r="Y19" s="8"/>
       <c r="Z19" s="19">

</xml_diff>

<commit_message>
Adding stats for minigun
</commit_message>
<xml_diff>
--- a/Documentation/Balance/Balance.xlsx
+++ b/Documentation/Balance/Balance.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Tank-Survivors\Documentation\Balance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C99EC3AD-0CDD-49A8-BA17-3774B8EB51F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D77A8F0E-BA7B-4C77-BA4C-2E0D5DC46E85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3744" yWindow="4956" windowWidth="23040" windowHeight="13644" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-17088" yWindow="3828" windowWidth="23040" windowHeight="13644" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -796,8 +796,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AG98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="V9" sqref="V9"/>
+    <sheetView tabSelected="1" topLeftCell="C9" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1815,9 +1815,11 @@
         <v>12</v>
       </c>
       <c r="D22" s="1">
-        <v>5</v>
-      </c>
-      <c r="E22" s="1"/>
+        <v>2</v>
+      </c>
+      <c r="E22" s="1">
+        <v>1</v>
+      </c>
       <c r="F22" s="1">
         <v>1</v>
       </c>
@@ -1852,7 +1854,7 @@
       <c r="Y22" s="1"/>
       <c r="Z22" s="18">
         <f t="shared" ref="Z22:Z28" si="2">SUM(D22:J22,L22:P22,R22:Y22)</f>
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="AA22" s="1" t="s">
         <v>12</v>
@@ -1866,13 +1868,15 @@
         <v>24</v>
       </c>
       <c r="D23" s="1">
-        <v>0.2</v>
+        <v>0.25</v>
       </c>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
-      <c r="I23" s="1"/>
+      <c r="I23" s="1">
+        <v>-0.05</v>
+      </c>
       <c r="J23" s="1"/>
       <c r="K23" s="1" t="s">
         <v>90</v>
@@ -2019,17 +2023,11 @@
       <c r="D26" s="13">
         <v>3</v>
       </c>
-      <c r="E26" s="1">
-        <v>1</v>
-      </c>
+      <c r="E26" s="1"/>
       <c r="F26" s="1"/>
-      <c r="G26" s="1">
-        <v>1</v>
-      </c>
+      <c r="G26" s="1"/>
       <c r="H26" s="1"/>
-      <c r="I26" s="13">
-        <v>1</v>
-      </c>
+      <c r="I26" s="13"/>
       <c r="J26" s="1"/>
       <c r="K26" s="1" t="s">
         <v>90</v>
@@ -2060,7 +2058,7 @@
       <c r="Y26" s="1"/>
       <c r="Z26" s="18">
         <f t="shared" si="2"/>
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="AA26" s="1" t="s">
         <v>34</v>
@@ -2074,7 +2072,7 @@
         <v>35</v>
       </c>
       <c r="D27" s="13">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E27" s="1">
         <v>1</v>
@@ -2113,7 +2111,7 @@
       <c r="Y27" s="1"/>
       <c r="Z27" s="18">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AA27" s="1" t="s">
         <v>35</v>
@@ -2180,11 +2178,13 @@
       </c>
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
-      <c r="G29" s="1"/>
+      <c r="G29" s="1">
+        <v>5</v>
+      </c>
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
       <c r="J29" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="K29" s="1" t="s">
         <v>90</v>
@@ -2208,8 +2208,8 @@
       <c r="X29" s="1"/>
       <c r="Y29" s="1"/>
       <c r="Z29" s="18">
-        <f>SUM(D29:J29,L29:P29,R29:Y29)*1.5</f>
-        <v>40.5</v>
+        <f>SUM(D29:J29,L29:P29,R29:Y29)</f>
+        <v>35</v>
       </c>
       <c r="AA29" s="1" t="s">
         <v>30</v>

</xml_diff>

<commit_message>
Added all stats for minigun
</commit_message>
<xml_diff>
--- a/Documentation/Balance/Balance.xlsx
+++ b/Documentation/Balance/Balance.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Tank-Survivors\Documentation\Balance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D77A8F0E-BA7B-4C77-BA4C-2E0D5DC46E85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C88B961A-10B1-427A-AF53-18C71CA7E92C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-17088" yWindow="3828" windowWidth="23040" windowHeight="13644" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-14712" yWindow="5124" windowWidth="23040" windowHeight="13644" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -796,8 +796,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AG98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C9" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+    <sheetView tabSelected="1" topLeftCell="M9" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="Z28" sqref="Z28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1815,7 +1815,7 @@
         <v>12</v>
       </c>
       <c r="D22" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E22" s="1">
         <v>1</v>
@@ -1833,7 +1833,7 @@
       <c r="L22" s="1"/>
       <c r="M22" s="1"/>
       <c r="N22" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O22" s="1"/>
       <c r="P22" s="1"/>
@@ -1843,18 +1843,18 @@
       <c r="R22" s="1"/>
       <c r="S22" s="1"/>
       <c r="T22" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="U22" s="1"/>
       <c r="V22" s="1"/>
       <c r="W22" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="X22" s="1"/>
       <c r="Y22" s="1"/>
       <c r="Z22" s="18">
         <f t="shared" ref="Z22:Z28" si="2">SUM(D22:J22,L22:P22,R22:Y22)</f>
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="AA22" s="1" t="s">
         <v>12</v>
@@ -1875,7 +1875,7 @@
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
       <c r="I23" s="1">
-        <v>-0.05</v>
+        <v>-0.03</v>
       </c>
       <c r="J23" s="1"/>
       <c r="K23" s="1" t="s">
@@ -1884,7 +1884,9 @@
       <c r="L23" s="1"/>
       <c r="M23" s="1"/>
       <c r="N23" s="1"/>
-      <c r="O23" s="1"/>
+      <c r="O23" s="1">
+        <v>-0.03</v>
+      </c>
       <c r="P23" s="1"/>
       <c r="Q23" s="1" t="s">
         <v>90</v>
@@ -1893,7 +1895,7 @@
       <c r="S23" s="1"/>
       <c r="T23" s="1"/>
       <c r="U23" s="1">
-        <v>-0.05</v>
+        <v>-0.03</v>
       </c>
       <c r="V23" s="1"/>
       <c r="W23" s="1"/>
@@ -1901,7 +1903,7 @@
       <c r="Y23" s="1"/>
       <c r="Z23" s="18">
         <f t="shared" si="2"/>
-        <v>0.15000000000000002</v>
+        <v>0.16</v>
       </c>
       <c r="AA23" s="1" t="s">
         <v>24</v>
@@ -1984,7 +1986,9 @@
         <v>90</v>
       </c>
       <c r="L25" s="1"/>
-      <c r="M25" s="1"/>
+      <c r="M25" s="1">
+        <v>30</v>
+      </c>
       <c r="N25" s="1"/>
       <c r="O25" s="1"/>
       <c r="P25" s="1">
@@ -2004,10 +2008,12 @@
       <c r="X25" s="1">
         <v>40</v>
       </c>
-      <c r="Y25" s="1"/>
+      <c r="Y25" s="1">
+        <v>40</v>
+      </c>
       <c r="Z25" s="18">
         <f t="shared" si="2"/>
-        <v>230</v>
+        <v>300</v>
       </c>
       <c r="AA25" s="1" t="s">
         <v>33</v>
@@ -2033,32 +2039,24 @@
         <v>90</v>
       </c>
       <c r="L26" s="1"/>
-      <c r="M26" s="1">
-        <v>2</v>
-      </c>
+      <c r="M26" s="1"/>
       <c r="N26" s="1"/>
-      <c r="O26" s="1">
-        <v>2</v>
-      </c>
+      <c r="O26" s="1"/>
       <c r="P26" s="1"/>
       <c r="Q26" s="1" t="s">
         <v>90</v>
       </c>
       <c r="R26" s="1"/>
-      <c r="S26" s="1">
-        <v>2</v>
-      </c>
+      <c r="S26" s="1"/>
       <c r="T26" s="1"/>
       <c r="U26" s="1"/>
-      <c r="V26" s="1">
-        <v>2</v>
-      </c>
+      <c r="V26" s="1"/>
       <c r="W26" s="1"/>
       <c r="X26" s="1"/>
       <c r="Y26" s="1"/>
       <c r="Z26" s="18">
         <f t="shared" si="2"/>
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="AA26" s="1" t="s">
         <v>34</v>
@@ -2125,7 +2123,7 @@
         <v>36</v>
       </c>
       <c r="D28" s="13">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
@@ -2139,7 +2137,9 @@
         <v>90</v>
       </c>
       <c r="L28" s="1"/>
-      <c r="M28" s="1"/>
+      <c r="M28" s="1">
+        <v>1</v>
+      </c>
       <c r="N28" s="1"/>
       <c r="O28" s="1"/>
       <c r="P28" s="1"/>
@@ -2147,20 +2147,22 @@
         <v>90</v>
       </c>
       <c r="R28" s="1"/>
-      <c r="S28" s="1"/>
+      <c r="S28" s="1">
+        <v>1</v>
+      </c>
       <c r="T28" s="1"/>
       <c r="U28" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="V28" s="1"/>
       <c r="W28" s="1"/>
       <c r="X28" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Y28" s="1"/>
       <c r="Z28" s="18">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AA28" s="1" t="s">
         <v>36</v>
@@ -2248,17 +2250,21 @@
       </c>
       <c r="R30" s="8"/>
       <c r="S30" s="8">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="T30" s="8"/>
       <c r="U30" s="8"/>
-      <c r="V30" s="8"/>
+      <c r="V30" s="8">
+        <v>3</v>
+      </c>
       <c r="W30" s="8"/>
       <c r="X30" s="8"/>
-      <c r="Y30" s="8"/>
+      <c r="Y30" s="8">
+        <v>5</v>
+      </c>
       <c r="Z30" s="18">
         <f>SUM(D30:J30,L30:P30,R30:Y30)</f>
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="AA30" s="8" t="s">
         <v>31</v>

</xml_diff>

<commit_message>
Add stats for railgun
</commit_message>
<xml_diff>
--- a/Documentation/Balance/Balance.xlsx
+++ b/Documentation/Balance/Balance.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Tank-Survivors\Documentation\Balance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C88B961A-10B1-427A-AF53-18C71CA7E92C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8EE1650-90C9-4019-946A-1044712B73D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-14712" yWindow="5124" windowWidth="23040" windowHeight="13644" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-16464" yWindow="6708" windowWidth="23040" windowHeight="13644" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="91">
   <si>
     <t>Здоровье</t>
   </si>
@@ -85,9 +85,6 @@
     <t>Дальность атаки</t>
   </si>
   <si>
-    <t>Снаряд</t>
-  </si>
-  <si>
     <t>Скорость снаряда</t>
   </si>
   <si>
@@ -113,9 +110,6 @@
   </si>
   <si>
     <t>Fire Range</t>
-  </si>
-  <si>
-    <t>Projectile</t>
   </si>
   <si>
     <t>Projectile speed</t>
@@ -796,8 +790,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AG98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M9" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="Z28" sqref="Z28"/>
+    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="J44" sqref="J44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -814,74 +808,74 @@
     <row r="1" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:27" x14ac:dyDescent="0.3">
       <c r="B2" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C2" s="3"/>
       <c r="E2" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="H2" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="I2" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="J2" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="K2" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="L2" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="M2" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="N2" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="O2" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="N2" s="3" t="s">
+      <c r="P2" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="O2" s="3" t="s">
+      <c r="Q2" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="P2" s="3" t="s">
+      <c r="R2" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="Q2" s="3" t="s">
+      <c r="S2" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="R2" s="3" t="s">
+      <c r="T2" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="S2" s="3" t="s">
+      <c r="U2" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="T2" s="3" t="s">
+      <c r="V2" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="U2" s="3" t="s">
+      <c r="W2" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="V2" s="3" t="s">
+      <c r="X2" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="W2" s="3" t="s">
+      <c r="Y2" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="X2" s="3" t="s">
+      <c r="Z2" s="4" t="s">
         <v>87</v>
-      </c>
-      <c r="Y2" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="Z2" s="4" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.3">
@@ -1159,79 +1153,79 @@
     <row r="9" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
       <c r="B9" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
       <c r="E9" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="G9" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="F9" s="3" t="s">
+      <c r="H9" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="G9" s="3" t="s">
+      <c r="I9" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="H9" s="3" t="s">
+      <c r="J9" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="I9" s="3" t="s">
+      <c r="K9" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="J9" s="3" t="s">
+      <c r="L9" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="K9" s="3" t="s">
+      <c r="M9" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="L9" s="3" t="s">
+      <c r="N9" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="M9" s="3" t="s">
+      <c r="O9" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="N9" s="3" t="s">
+      <c r="P9" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="O9" s="3" t="s">
+      <c r="Q9" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="P9" s="3" t="s">
+      <c r="R9" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="Q9" s="3" t="s">
+      <c r="S9" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="R9" s="3" t="s">
+      <c r="T9" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="S9" s="3" t="s">
+      <c r="U9" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="T9" s="3" t="s">
+      <c r="V9" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="U9" s="3" t="s">
+      <c r="W9" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="V9" s="3" t="s">
+      <c r="X9" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="W9" s="3" t="s">
+      <c r="Y9" s="3" t="s">
         <v>86</v>
-      </c>
-      <c r="X9" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="Y9" s="3" t="s">
-        <v>88</v>
       </c>
       <c r="Z9" s="4"/>
     </row>
     <row r="10" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
       <c r="B10" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>12</v>
@@ -1252,7 +1246,7 @@
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
       <c r="K10" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="L10" s="1"/>
       <c r="M10" s="1"/>
@@ -1264,7 +1258,7 @@
         <v>4</v>
       </c>
       <c r="Q10" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="R10" s="1"/>
       <c r="S10" s="1">
@@ -1293,7 +1287,7 @@
         <v>13</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D11" s="1">
         <v>1</v>
@@ -1307,7 +1301,7 @@
       </c>
       <c r="J11" s="1"/>
       <c r="K11" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="L11" s="1"/>
       <c r="M11" s="1"/>
@@ -1317,7 +1311,7 @@
       </c>
       <c r="P11" s="1"/>
       <c r="Q11" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="R11" s="1">
         <v>-0.2</v>
@@ -1336,7 +1330,7 @@
         <v>0.29999999999999993</v>
       </c>
       <c r="AA11" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:27" x14ac:dyDescent="0.3">
@@ -1360,17 +1354,17 @@
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
       <c r="K12" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="L12" s="1" t="s">
         <v>90</v>
-      </c>
-      <c r="L12" s="1" t="s">
-        <v>92</v>
       </c>
       <c r="M12" s="1"/>
       <c r="N12" s="1"/>
       <c r="O12" s="1"/>
       <c r="P12" s="1"/>
       <c r="Q12" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="R12" s="1">
         <v>15</v>
@@ -1399,7 +1393,7 @@
         <v>15</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D13" s="1">
         <v>100</v>
@@ -1415,7 +1409,7 @@
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
       <c r="K13" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="M13" s="1">
         <v>20</v>
@@ -1426,7 +1420,7 @@
         <v>30</v>
       </c>
       <c r="Q13" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="R13" s="1"/>
       <c r="S13" s="1"/>
@@ -1445,7 +1439,7 @@
         <v>270</v>
       </c>
       <c r="AA13" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:27" x14ac:dyDescent="0.3">
@@ -1453,7 +1447,7 @@
         <v>16</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D14" s="1">
         <v>14</v>
@@ -1465,7 +1459,7 @@
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
       <c r="K14" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="L14" s="1"/>
       <c r="M14" s="1"/>
@@ -1473,7 +1467,7 @@
       <c r="O14" s="1"/>
       <c r="P14" s="1"/>
       <c r="Q14" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="R14" s="1"/>
       <c r="S14" s="1"/>
@@ -1488,15 +1482,15 @@
         <v>14</v>
       </c>
       <c r="AA14" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="15" spans="1:27" x14ac:dyDescent="0.3">
       <c r="B15" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D15" s="1">
         <v>8</v>
@@ -1510,7 +1504,7 @@
         <v>5</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="L15" s="1"/>
       <c r="M15" s="1">
@@ -1520,7 +1514,7 @@
       <c r="O15" s="1"/>
       <c r="P15" s="1"/>
       <c r="Q15" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="R15" s="1"/>
       <c r="S15" s="1"/>
@@ -1537,15 +1531,15 @@
         <v>22</v>
       </c>
       <c r="AA15" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="16" spans="1:27" x14ac:dyDescent="0.3">
       <c r="B16" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D16" s="1">
         <v>2</v>
@@ -1559,7 +1553,7 @@
       <c r="I16" s="1"/>
       <c r="J16" s="22"/>
       <c r="K16" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="L16" s="1"/>
       <c r="M16" s="1"/>
@@ -1569,7 +1563,7 @@
       </c>
       <c r="P16" s="1"/>
       <c r="Q16" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="R16" s="1"/>
       <c r="S16" s="1">
@@ -1588,15 +1582,15 @@
         <v>6</v>
       </c>
       <c r="AA16" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="17" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B17" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D17" s="1">
         <v>5</v>
@@ -1610,17 +1604,17 @@
       </c>
       <c r="J17" s="22"/>
       <c r="K17" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="L17" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="M17" s="1"/>
       <c r="N17" s="1"/>
       <c r="O17" s="1"/>
       <c r="P17" s="1"/>
       <c r="Q17" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="R17" s="1"/>
       <c r="S17" s="1"/>
@@ -1637,15 +1631,15 @@
         <v>25</v>
       </c>
       <c r="AA17" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="18" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B18" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D18" s="13">
         <v>14</v>
@@ -1659,7 +1653,7 @@
         <v>3</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="L18" s="1"/>
       <c r="M18" s="1"/>
@@ -1669,7 +1663,7 @@
       <c r="O18" s="1"/>
       <c r="P18" s="1"/>
       <c r="Q18" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="R18" s="1"/>
       <c r="S18" s="1"/>
@@ -1686,15 +1680,15 @@
         <v>25</v>
       </c>
       <c r="AA18" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="19" spans="2:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B19" s="7" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D19" s="21">
         <f>D11 * 125%</f>
@@ -1707,7 +1701,7 @@
       <c r="I19" s="8"/>
       <c r="J19" s="8"/>
       <c r="K19" s="8" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="L19" s="8"/>
       <c r="M19" s="8"/>
@@ -1715,7 +1709,7 @@
       <c r="O19" s="8"/>
       <c r="P19" s="8"/>
       <c r="Q19" s="8" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="R19" s="8"/>
       <c r="S19" s="8"/>
@@ -1732,78 +1726,78 @@
         <v>0.37499999999999989</v>
       </c>
       <c r="AA19" s="8" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="20" spans="2:27" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="21" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B21" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
       <c r="E21" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="G21" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="F21" s="3" t="s">
+      <c r="H21" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="G21" s="3" t="s">
+      <c r="I21" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="H21" s="3" t="s">
+      <c r="J21" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="I21" s="3" t="s">
+      <c r="K21" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="J21" s="3" t="s">
+      <c r="L21" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="K21" s="3" t="s">
+      <c r="M21" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="L21" s="3" t="s">
+      <c r="N21" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="M21" s="3" t="s">
+      <c r="O21" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="N21" s="3" t="s">
+      <c r="P21" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="O21" s="3" t="s">
+      <c r="Q21" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="P21" s="3" t="s">
+      <c r="R21" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="Q21" s="3" t="s">
+      <c r="S21" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="R21" s="3" t="s">
+      <c r="T21" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="S21" s="3" t="s">
+      <c r="U21" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="T21" s="3" t="s">
+      <c r="V21" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="U21" s="3" t="s">
+      <c r="W21" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="V21" s="3" t="s">
+      <c r="X21" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="W21" s="3" t="s">
+      <c r="Y21" s="3" t="s">
         <v>86</v>
-      </c>
-      <c r="X21" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="Y21" s="3" t="s">
-        <v>88</v>
       </c>
       <c r="Z21" s="20"/>
     </row>
@@ -1828,7 +1822,7 @@
       <c r="I22" s="1"/>
       <c r="J22" s="1"/>
       <c r="K22" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="L22" s="1"/>
       <c r="M22" s="1"/>
@@ -1838,7 +1832,7 @@
       <c r="O22" s="1"/>
       <c r="P22" s="1"/>
       <c r="Q22" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="R22" s="1"/>
       <c r="S22" s="1"/>
@@ -1865,7 +1859,7 @@
         <v>13</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D23" s="1">
         <v>0.25</v>
@@ -1879,7 +1873,7 @@
       </c>
       <c r="J23" s="1"/>
       <c r="K23" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="L23" s="1"/>
       <c r="M23" s="1"/>
@@ -1889,7 +1883,7 @@
       </c>
       <c r="P23" s="1"/>
       <c r="Q23" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="R23" s="1"/>
       <c r="S23" s="1"/>
@@ -1906,7 +1900,7 @@
         <v>0.16</v>
       </c>
       <c r="AA23" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="24" spans="2:27" x14ac:dyDescent="0.3">
@@ -1930,7 +1924,7 @@
       <c r="I24" s="1"/>
       <c r="J24" s="1"/>
       <c r="K24" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="L24" s="1">
         <v>20</v>
@@ -1942,7 +1936,7 @@
       <c r="O24" s="1"/>
       <c r="P24" s="1"/>
       <c r="Q24" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="R24" s="1"/>
       <c r="S24" s="1"/>
@@ -1969,7 +1963,7 @@
         <v>15</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D25" s="13">
         <v>100</v>
@@ -1983,7 +1977,7 @@
       <c r="I25" s="1"/>
       <c r="J25" s="1"/>
       <c r="K25" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="L25" s="1"/>
       <c r="M25" s="1">
@@ -1995,7 +1989,7 @@
         <v>30</v>
       </c>
       <c r="Q25" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="R25" s="1">
         <v>40</v>
@@ -2016,7 +2010,7 @@
         <v>300</v>
       </c>
       <c r="AA25" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="26" spans="2:27" x14ac:dyDescent="0.3">
@@ -2024,7 +2018,7 @@
         <v>16</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D26" s="13">
         <v>3</v>
@@ -2036,7 +2030,7 @@
       <c r="I26" s="13"/>
       <c r="J26" s="1"/>
       <c r="K26" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="L26" s="1"/>
       <c r="M26" s="1"/>
@@ -2044,7 +2038,7 @@
       <c r="O26" s="1"/>
       <c r="P26" s="1"/>
       <c r="Q26" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="R26" s="1"/>
       <c r="S26" s="1"/>
@@ -2059,15 +2053,15 @@
         <v>3</v>
       </c>
       <c r="AA26" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="27" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B27" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D27" s="13">
         <v>4</v>
@@ -2083,7 +2077,7 @@
       </c>
       <c r="J27" s="1"/>
       <c r="K27" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="L27" s="1">
         <v>1</v>
@@ -2095,7 +2089,7 @@
         <v>1</v>
       </c>
       <c r="Q27" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="R27" s="1"/>
       <c r="S27" s="1"/>
@@ -2112,15 +2106,15 @@
         <v>9</v>
       </c>
       <c r="AA27" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="28" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B28" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D28" s="13">
         <v>4</v>
@@ -2134,7 +2128,7 @@
         <v>1</v>
       </c>
       <c r="K28" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="L28" s="1"/>
       <c r="M28" s="1">
@@ -2144,7 +2138,7 @@
       <c r="O28" s="1"/>
       <c r="P28" s="1"/>
       <c r="Q28" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="R28" s="1"/>
       <c r="S28" s="1">
@@ -2165,15 +2159,15 @@
         <v>9</v>
       </c>
       <c r="AA28" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="29" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B29" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D29" s="13">
         <v>20</v>
@@ -2189,7 +2183,7 @@
         <v>5</v>
       </c>
       <c r="K29" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="L29" s="1"/>
       <c r="M29" s="1"/>
@@ -2197,7 +2191,7 @@
       <c r="O29" s="1"/>
       <c r="P29" s="1"/>
       <c r="Q29" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="R29" s="1">
         <v>5</v>
@@ -2214,15 +2208,15 @@
         <v>35</v>
       </c>
       <c r="AA29" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="30" spans="2:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B30" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D30" s="8">
         <v>10</v>
@@ -2236,7 +2230,7 @@
       <c r="I30" s="8"/>
       <c r="J30" s="8"/>
       <c r="K30" s="8" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="L30" s="8"/>
       <c r="M30" s="8"/>
@@ -2246,7 +2240,7 @@
       </c>
       <c r="P30" s="8"/>
       <c r="Q30" s="8" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="R30" s="8"/>
       <c r="S30" s="8">
@@ -2267,78 +2261,78 @@
         <v>25</v>
       </c>
       <c r="AA30" s="8" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="31" spans="2:27" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="32" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B32" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C32" s="3"/>
       <c r="D32" s="3"/>
       <c r="E32" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="F32" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="G32" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="F32" s="3" t="s">
+      <c r="H32" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="G32" s="3" t="s">
+      <c r="I32" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="H32" s="3" t="s">
+      <c r="J32" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="I32" s="3" t="s">
+      <c r="K32" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="J32" s="3" t="s">
+      <c r="L32" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="K32" s="3" t="s">
+      <c r="M32" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="L32" s="3" t="s">
+      <c r="N32" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="M32" s="3" t="s">
+      <c r="O32" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="N32" s="3" t="s">
+      <c r="P32" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="O32" s="3" t="s">
+      <c r="Q32" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="P32" s="3" t="s">
+      <c r="R32" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="Q32" s="3" t="s">
+      <c r="S32" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="R32" s="3" t="s">
+      <c r="T32" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="S32" s="3" t="s">
+      <c r="U32" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="T32" s="3" t="s">
+      <c r="V32" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="U32" s="3" t="s">
+      <c r="W32" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="V32" s="3" t="s">
+      <c r="X32" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="W32" s="3" t="s">
+      <c r="Y32" s="3" t="s">
         <v>86</v>
-      </c>
-      <c r="X32" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="Y32" s="3" t="s">
-        <v>88</v>
       </c>
       <c r="Z32" s="20"/>
     </row>
@@ -2365,7 +2359,7 @@
         <v>5</v>
       </c>
       <c r="K33" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="L33" s="1"/>
       <c r="M33" s="1"/>
@@ -2373,7 +2367,7 @@
       <c r="O33" s="1"/>
       <c r="P33" s="1"/>
       <c r="Q33" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="R33" s="1"/>
       <c r="S33" s="1"/>
@@ -2396,7 +2390,7 @@
         <v>13</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D34" s="13">
         <v>2</v>
@@ -2414,7 +2408,7 @@
       </c>
       <c r="J34" s="1"/>
       <c r="K34" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="L34" s="1"/>
       <c r="M34" s="1"/>
@@ -2422,7 +2416,7 @@
       <c r="O34" s="1"/>
       <c r="P34" s="1"/>
       <c r="Q34" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="R34" s="1"/>
       <c r="S34" s="1"/>
@@ -2437,7 +2431,7 @@
         <v>1.4000000000000001</v>
       </c>
       <c r="AA34" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="35" spans="2:27" x14ac:dyDescent="0.3">
@@ -2459,7 +2453,7 @@
         <v>20</v>
       </c>
       <c r="K35" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="L35" s="1"/>
       <c r="M35" s="1"/>
@@ -2467,7 +2461,7 @@
       <c r="O35" s="1"/>
       <c r="P35" s="1"/>
       <c r="Q35" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="R35" s="1"/>
       <c r="S35" s="1"/>
@@ -2490,7 +2484,7 @@
         <v>15</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D36" s="13">
         <v>100</v>
@@ -2502,7 +2496,7 @@
       <c r="I36" s="1"/>
       <c r="J36" s="1"/>
       <c r="K36" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="L36" s="1"/>
       <c r="M36" s="1"/>
@@ -2510,7 +2504,7 @@
       <c r="O36" s="1"/>
       <c r="P36" s="1"/>
       <c r="Q36" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="R36" s="1"/>
       <c r="S36" s="1"/>
@@ -2525,15 +2519,15 @@
         <v>100</v>
       </c>
       <c r="AA36" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="37" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B37" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D37" s="13">
         <v>3</v>
@@ -2549,7 +2543,7 @@
       <c r="I37" s="1"/>
       <c r="J37" s="1"/>
       <c r="K37" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="L37" s="1"/>
       <c r="M37" s="1"/>
@@ -2557,7 +2551,7 @@
       <c r="O37" s="1"/>
       <c r="P37" s="1"/>
       <c r="Q37" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="R37" s="1"/>
       <c r="S37" s="1"/>
@@ -2572,15 +2566,15 @@
         <v>7</v>
       </c>
       <c r="AA37" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="38" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B38" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D38" s="13">
         <v>2</v>
@@ -2596,7 +2590,7 @@
       <c r="I38" s="1"/>
       <c r="J38" s="1"/>
       <c r="K38" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="L38" s="1"/>
       <c r="M38" s="1"/>
@@ -2604,7 +2598,7 @@
       <c r="O38" s="1"/>
       <c r="P38" s="1"/>
       <c r="Q38" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="R38" s="1"/>
       <c r="S38" s="1"/>
@@ -2619,15 +2613,15 @@
         <v>4</v>
       </c>
       <c r="AA38" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="39" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B39" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D39" s="13">
         <v>1</v>
@@ -2643,7 +2637,7 @@
       <c r="I39" s="1"/>
       <c r="J39" s="1"/>
       <c r="K39" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="L39" s="1"/>
       <c r="M39" s="1"/>
@@ -2651,7 +2645,7 @@
       <c r="O39" s="1"/>
       <c r="P39" s="1"/>
       <c r="Q39" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="R39" s="1"/>
       <c r="S39" s="1"/>
@@ -2666,15 +2660,15 @@
         <v>2</v>
       </c>
       <c r="AA39" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="40" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B40" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D40" s="13">
         <v>20</v>
@@ -2690,7 +2684,7 @@
       <c r="I40" s="1"/>
       <c r="J40" s="1"/>
       <c r="K40" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="L40" s="1"/>
       <c r="M40" s="1"/>
@@ -2698,7 +2692,7 @@
       <c r="O40" s="1"/>
       <c r="P40" s="1"/>
       <c r="Q40" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="R40" s="1"/>
       <c r="S40" s="1"/>
@@ -2713,15 +2707,15 @@
         <v>30</v>
       </c>
       <c r="AA40" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="41" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B41" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D41" s="13">
         <v>10</v>
@@ -2737,7 +2731,7 @@
       <c r="I41" s="1"/>
       <c r="J41" s="1"/>
       <c r="K41" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="L41" s="1"/>
       <c r="M41" s="1"/>
@@ -2745,7 +2739,7 @@
       <c r="O41" s="1"/>
       <c r="P41" s="1"/>
       <c r="Q41" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="R41" s="1"/>
       <c r="S41" s="1"/>
@@ -2760,15 +2754,15 @@
         <v>20</v>
       </c>
       <c r="AA41" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="42" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B42" s="24" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C42" s="25" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D42" s="26">
         <v>20</v>
@@ -2780,7 +2774,7 @@
       <c r="I42" s="25"/>
       <c r="J42" s="25"/>
       <c r="K42" s="25" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="L42" s="25">
         <v>5</v>
@@ -2794,7 +2788,7 @@
         <v>5</v>
       </c>
       <c r="Q42" s="25" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="R42" s="25"/>
       <c r="S42" s="25"/>
@@ -2809,15 +2803,15 @@
         <v>35</v>
       </c>
       <c r="AA42" s="25" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="43" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B43" s="24" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C43" s="25" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D43" s="26">
         <v>5</v>
@@ -2829,7 +2823,7 @@
       <c r="I43" s="25"/>
       <c r="J43" s="25"/>
       <c r="K43" s="25" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="L43" s="25">
         <v>-1</v>
@@ -2843,7 +2837,7 @@
         <v>-1</v>
       </c>
       <c r="Q43" s="25" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="R43" s="25"/>
       <c r="S43" s="25"/>
@@ -2858,15 +2852,15 @@
         <v>2</v>
       </c>
       <c r="AA43" s="25" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="44" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B44" s="24" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C44" s="25" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D44" s="26">
         <v>1</v>
@@ -2878,7 +2872,7 @@
       <c r="I44" s="25"/>
       <c r="J44" s="25"/>
       <c r="K44" s="25" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="L44" s="25"/>
       <c r="M44" s="25">
@@ -2888,7 +2882,7 @@
       <c r="O44" s="25"/>
       <c r="P44" s="25"/>
       <c r="Q44" s="25" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="R44" s="25"/>
       <c r="S44" s="25"/>
@@ -2903,15 +2897,15 @@
         <v>2</v>
       </c>
       <c r="AA44" s="25" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="45" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B45" s="24" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C45" s="25" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D45" s="26">
         <v>3</v>
@@ -2923,7 +2917,7 @@
       <c r="I45" s="25"/>
       <c r="J45" s="25"/>
       <c r="K45" s="25" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="L45" s="25"/>
       <c r="M45" s="25">
@@ -2935,7 +2929,7 @@
       </c>
       <c r="P45" s="25"/>
       <c r="Q45" s="25" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="R45" s="25"/>
       <c r="S45" s="25"/>
@@ -2950,15 +2944,15 @@
         <v>5</v>
       </c>
       <c r="AA45" s="25" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="46" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B46" s="24" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C46" s="25" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D46" s="26">
         <v>0.5</v>
@@ -2970,7 +2964,7 @@
       <c r="I46" s="25"/>
       <c r="J46" s="25"/>
       <c r="K46" s="25" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="L46" s="25"/>
       <c r="M46" s="25"/>
@@ -2980,7 +2974,7 @@
       </c>
       <c r="P46" s="25"/>
       <c r="Q46" s="25" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="R46" s="25"/>
       <c r="S46" s="25"/>
@@ -2995,15 +2989,15 @@
         <v>0.3</v>
       </c>
       <c r="AA46" s="25" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="47" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B47" s="24" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C47" s="25" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D47" s="26">
         <v>0</v>
@@ -3015,7 +3009,7 @@
       <c r="I47" s="25"/>
       <c r="J47" s="25"/>
       <c r="K47" s="25" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="L47" s="25"/>
       <c r="M47" s="25"/>
@@ -3023,7 +3017,7 @@
       <c r="O47" s="25"/>
       <c r="P47" s="25"/>
       <c r="Q47" s="25" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="R47" s="22">
         <v>1</v>
@@ -3046,15 +3040,15 @@
         <v>4</v>
       </c>
       <c r="AA47" s="25" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="48" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B48" s="5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D48" s="13">
         <v>5</v>
@@ -3066,7 +3060,7 @@
       <c r="I48" s="1"/>
       <c r="J48" s="1"/>
       <c r="K48" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="L48" s="1"/>
       <c r="M48" s="1"/>
@@ -3074,7 +3068,7 @@
       <c r="O48" s="1"/>
       <c r="P48" s="1"/>
       <c r="Q48" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="R48" s="22">
         <v>5</v>
@@ -3097,15 +3091,15 @@
         <v>25</v>
       </c>
       <c r="AA48" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="49" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B49" s="5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D49" s="13">
         <v>0.1</v>
@@ -3117,7 +3111,7 @@
       <c r="I49" s="1"/>
       <c r="J49" s="1"/>
       <c r="K49" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="L49" s="1"/>
       <c r="M49" s="1"/>
@@ -3125,7 +3119,7 @@
       <c r="O49" s="1"/>
       <c r="P49" s="1"/>
       <c r="Q49" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="R49" s="22"/>
       <c r="S49" s="1">
@@ -3148,15 +3142,15 @@
         <v>5.0000000000000017E-2</v>
       </c>
       <c r="AA49" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="50" spans="2:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B50" s="7" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C50" s="8" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D50" s="8">
         <v>2</v>
@@ -3168,7 +3162,7 @@
       <c r="I50" s="8"/>
       <c r="J50" s="8"/>
       <c r="K50" s="8" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="L50" s="8"/>
       <c r="M50" s="8"/>
@@ -3176,7 +3170,7 @@
       <c r="O50" s="8"/>
       <c r="P50" s="8"/>
       <c r="Q50" s="8" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="R50" s="29">
         <v>1</v>
@@ -3199,78 +3193,78 @@
         <v>6</v>
       </c>
       <c r="AA50" s="8" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="51" spans="2:27" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="52" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B52" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C52" s="3"/>
       <c r="D52" s="3"/>
       <c r="E52" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="F52" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="G52" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="F52" s="3" t="s">
+      <c r="H52" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="G52" s="3" t="s">
+      <c r="I52" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="H52" s="3" t="s">
+      <c r="J52" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="I52" s="3" t="s">
+      <c r="K52" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="J52" s="3" t="s">
+      <c r="L52" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="K52" s="3" t="s">
+      <c r="M52" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="L52" s="3" t="s">
+      <c r="N52" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="M52" s="3" t="s">
+      <c r="O52" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="N52" s="3" t="s">
+      <c r="P52" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="O52" s="3" t="s">
+      <c r="Q52" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="P52" s="3" t="s">
+      <c r="R52" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="Q52" s="3" t="s">
+      <c r="S52" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="R52" s="3" t="s">
+      <c r="T52" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="S52" s="3" t="s">
+      <c r="U52" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="T52" s="3" t="s">
+      <c r="V52" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="U52" s="3" t="s">
+      <c r="W52" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="V52" s="3" t="s">
+      <c r="X52" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="W52" s="3" t="s">
+      <c r="Y52" s="3" t="s">
         <v>86</v>
-      </c>
-      <c r="X52" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="Y52" s="3" t="s">
-        <v>88</v>
       </c>
       <c r="Z52" s="20"/>
     </row>
@@ -3299,7 +3293,7 @@
         <v>1</v>
       </c>
       <c r="K53" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="L53" s="1"/>
       <c r="M53" s="22">
@@ -3311,7 +3305,7 @@
       </c>
       <c r="P53" s="1"/>
       <c r="Q53" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="R53" s="1">
         <v>3</v>
@@ -3344,7 +3338,7 @@
         <v>13</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D54" s="1">
         <v>2</v>
@@ -3353,7 +3347,7 @@
         <v>0.2</v>
       </c>
       <c r="F54" s="1">
-        <v>-0.1</v>
+        <v>-0.2</v>
       </c>
       <c r="G54" s="1"/>
       <c r="H54" s="13">
@@ -3364,7 +3358,7 @@
       </c>
       <c r="J54" s="1"/>
       <c r="K54" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="L54" s="1">
         <v>-0.3</v>
@@ -3380,7 +3374,7 @@
       </c>
       <c r="P54" s="1"/>
       <c r="Q54" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="R54" s="1"/>
       <c r="S54" s="22">
@@ -3398,10 +3392,10 @@
       <c r="Y54" s="1"/>
       <c r="Z54" s="18">
         <f t="shared" ref="Z54:Z63" si="5">SUM(D54:J54,L54:P54,R54:Y54)</f>
-        <v>4.7</v>
+        <v>4.6000000000000005</v>
       </c>
       <c r="AA54" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="55" spans="2:27" x14ac:dyDescent="0.3">
@@ -3423,7 +3417,7 @@
       <c r="I55" s="1"/>
       <c r="J55" s="1"/>
       <c r="K55" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="L55" s="1"/>
       <c r="M55" s="1"/>
@@ -3433,7 +3427,7 @@
       <c r="O55" s="1"/>
       <c r="P55" s="1"/>
       <c r="Q55" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="R55" s="1"/>
       <c r="S55" s="1"/>
@@ -3458,10 +3452,10 @@
         <v>15</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D56" s="13">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="E56" s="1"/>
       <c r="F56" s="1"/>
@@ -3472,7 +3466,7 @@
       <c r="I56" s="1"/>
       <c r="J56" s="1"/>
       <c r="K56" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="L56" s="1"/>
       <c r="M56" s="1"/>
@@ -3482,7 +3476,7 @@
         <v>30</v>
       </c>
       <c r="Q56" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="R56" s="1"/>
       <c r="S56" s="1"/>
@@ -3496,10 +3490,10 @@
       <c r="Y56" s="1"/>
       <c r="Z56" s="18">
         <f t="shared" si="5"/>
-        <v>200</v>
+        <v>150</v>
       </c>
       <c r="AA56" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="57" spans="2:27" x14ac:dyDescent="0.3">
@@ -3507,7 +3501,7 @@
         <v>16</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D57" s="13">
         <v>10</v>
@@ -3517,11 +3511,9 @@
       <c r="G57" s="1"/>
       <c r="H57" s="1"/>
       <c r="I57" s="1"/>
-      <c r="J57" s="1">
-        <v>3</v>
-      </c>
+      <c r="J57" s="1"/>
       <c r="K57" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="L57" s="1"/>
       <c r="M57" s="1"/>
@@ -3529,129 +3521,135 @@
       <c r="O57" s="1"/>
       <c r="P57" s="1"/>
       <c r="Q57" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="R57" s="1">
-        <v>3</v>
-      </c>
+        <v>88</v>
+      </c>
+      <c r="R57" s="1"/>
       <c r="S57" s="1"/>
       <c r="T57" s="1"/>
       <c r="U57" s="1"/>
       <c r="V57" s="1"/>
-      <c r="W57" s="1">
-        <v>4</v>
-      </c>
+      <c r="W57" s="1"/>
       <c r="X57" s="1"/>
       <c r="Y57" s="1"/>
       <c r="Z57" s="18">
         <f t="shared" si="5"/>
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="AA57" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="58" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B58" s="5" t="s">
-        <v>17</v>
+        <v>62</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D58" s="1"/>
+        <v>59</v>
+      </c>
+      <c r="D58" s="13">
+        <v>1</v>
+      </c>
       <c r="E58" s="1"/>
       <c r="F58" s="1"/>
-      <c r="G58" s="1"/>
+      <c r="G58" s="1">
+        <v>0.5</v>
+      </c>
       <c r="H58" s="1"/>
       <c r="I58" s="1"/>
       <c r="J58" s="1"/>
       <c r="K58" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="L58" s="1"/>
       <c r="M58" s="1"/>
-      <c r="N58" s="1"/>
+      <c r="N58" s="22">
+        <v>1</v>
+      </c>
       <c r="O58" s="1"/>
       <c r="P58" s="1"/>
       <c r="Q58" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="R58" s="1"/>
       <c r="S58" s="1"/>
       <c r="T58" s="1"/>
-      <c r="U58" s="1"/>
-      <c r="V58" s="1"/>
+      <c r="U58" s="22">
+        <v>1</v>
+      </c>
+      <c r="V58" s="1">
+        <v>1</v>
+      </c>
       <c r="W58" s="1"/>
       <c r="X58" s="1"/>
       <c r="Y58" s="1"/>
       <c r="Z58" s="18">
-        <f t="shared" si="5"/>
-        <v>0</v>
+        <f>SUM(D58:J58,L58:P58,R58:Y58)</f>
+        <v>4.5</v>
       </c>
       <c r="AA58" s="1" t="s">
-        <v>27</v>
+        <v>59</v>
       </c>
     </row>
     <row r="59" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B59" s="5" t="s">
-        <v>64</v>
+        <v>20</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>61</v>
+        <v>29</v>
       </c>
       <c r="D59" s="13">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="E59" s="1"/>
       <c r="F59" s="1"/>
-      <c r="G59" s="1">
-        <v>0.5</v>
-      </c>
+      <c r="G59" s="1"/>
       <c r="H59" s="1"/>
       <c r="I59" s="1"/>
-      <c r="J59" s="1"/>
+      <c r="J59" s="1">
+        <v>2</v>
+      </c>
       <c r="K59" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="L59" s="1"/>
       <c r="M59" s="1"/>
-      <c r="N59" s="22">
-        <v>1</v>
-      </c>
+      <c r="N59" s="1"/>
       <c r="O59" s="1"/>
       <c r="P59" s="1"/>
       <c r="Q59" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="R59" s="1"/>
-      <c r="S59" s="1"/>
+        <v>88</v>
+      </c>
+      <c r="R59" s="1">
+        <v>2</v>
+      </c>
+      <c r="S59" s="1">
+        <v>3</v>
+      </c>
       <c r="T59" s="1"/>
-      <c r="U59" s="22">
-        <v>1</v>
-      </c>
-      <c r="V59" s="1">
-        <v>1</v>
-      </c>
+      <c r="U59" s="1"/>
+      <c r="V59" s="1"/>
       <c r="W59" s="1"/>
-      <c r="X59" s="1"/>
+      <c r="X59" s="1">
+        <v>3</v>
+      </c>
       <c r="Y59" s="1"/>
       <c r="Z59" s="18">
-        <f t="shared" si="5"/>
-        <v>4.5</v>
+        <f>SUM(D59:J59,L59:P59,R59:Y59)</f>
+        <v>25</v>
       </c>
       <c r="AA59" s="1" t="s">
-        <v>61</v>
+        <v>29</v>
       </c>
     </row>
     <row r="60" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B60" s="5" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="D60" s="13">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="E60" s="1"/>
       <c r="F60" s="1"/>
@@ -3660,7 +3658,7 @@
       <c r="I60" s="1"/>
       <c r="J60" s="1"/>
       <c r="K60" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="L60" s="1"/>
       <c r="M60" s="1"/>
@@ -3668,171 +3666,126 @@
       <c r="O60" s="1"/>
       <c r="P60" s="1"/>
       <c r="Q60" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="R60" s="1"/>
-      <c r="S60" s="1">
-        <v>5</v>
-      </c>
+      <c r="S60" s="1"/>
       <c r="T60" s="1"/>
-      <c r="U60" s="1"/>
+      <c r="U60" s="1">
+        <v>1</v>
+      </c>
       <c r="V60" s="1"/>
       <c r="W60" s="1"/>
-      <c r="X60" s="1">
-        <v>5</v>
-      </c>
+      <c r="X60" s="1"/>
       <c r="Y60" s="1"/>
       <c r="Z60" s="18">
-        <f t="shared" si="5"/>
-        <v>25</v>
+        <f>SUM(D60:J60,L60:P60,R60:Y60)</f>
+        <v>2</v>
       </c>
       <c r="AA60" s="1" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
     </row>
     <row r="61" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B61" s="5" t="s">
-        <v>19</v>
+        <v>63</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>36</v>
+        <v>60</v>
       </c>
       <c r="D61" s="13">
-        <v>1</v>
-      </c>
-      <c r="E61" s="1"/>
+        <v>0.2</v>
+      </c>
+      <c r="E61" s="1">
+        <v>-0.01</v>
+      </c>
       <c r="F61" s="1"/>
       <c r="G61" s="1"/>
       <c r="H61" s="1"/>
-      <c r="I61" s="1"/>
+      <c r="I61" s="1">
+        <v>-0.01</v>
+      </c>
       <c r="J61" s="1"/>
       <c r="K61" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="L61" s="1"/>
-      <c r="M61" s="1"/>
+        <v>88</v>
+      </c>
+      <c r="L61" s="1">
+        <v>-0.01</v>
+      </c>
+      <c r="M61" s="1">
+        <v>-0.01</v>
+      </c>
       <c r="N61" s="1"/>
-      <c r="O61" s="1"/>
-      <c r="P61" s="1"/>
+      <c r="O61" s="1">
+        <v>-0.01</v>
+      </c>
+      <c r="P61" s="1">
+        <v>-0.01</v>
+      </c>
       <c r="Q61" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="R61" s="1"/>
       <c r="S61" s="1"/>
       <c r="T61" s="1"/>
-      <c r="U61" s="1">
-        <v>1</v>
-      </c>
+      <c r="U61" s="1"/>
       <c r="V61" s="1"/>
-      <c r="W61" s="1"/>
+      <c r="W61" s="1">
+        <v>-0.02</v>
+      </c>
       <c r="X61" s="1"/>
       <c r="Y61" s="1"/>
       <c r="Z61" s="18">
-        <f t="shared" si="5"/>
-        <v>2</v>
+        <f>SUM(D61:J61,L61:P61,R61:Y61)</f>
+        <v>0.11999999999999995</v>
       </c>
       <c r="AA61" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="62" spans="2:27" x14ac:dyDescent="0.3">
-      <c r="B62" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="C62" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="D62" s="13">
-        <v>0.2</v>
-      </c>
-      <c r="E62" s="1">
-        <v>-0.03</v>
-      </c>
-      <c r="F62" s="1"/>
-      <c r="G62" s="1"/>
-      <c r="H62" s="1"/>
-      <c r="I62" s="1">
-        <v>-0.03</v>
-      </c>
-      <c r="J62" s="1"/>
-      <c r="K62" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="L62" s="1">
-        <v>-0.01</v>
-      </c>
-      <c r="M62" s="1">
-        <v>-0.01</v>
-      </c>
-      <c r="N62" s="1"/>
-      <c r="O62" s="1">
-        <v>-0.01</v>
-      </c>
-      <c r="P62" s="1">
-        <v>-0.02</v>
-      </c>
-      <c r="Q62" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="R62" s="1"/>
-      <c r="S62" s="1"/>
-      <c r="T62" s="1"/>
-      <c r="U62" s="1"/>
-      <c r="V62" s="1"/>
-      <c r="W62" s="1">
-        <v>-0.04</v>
-      </c>
-      <c r="X62" s="1"/>
-      <c r="Y62" s="1"/>
-      <c r="Z62" s="18">
-        <f t="shared" si="5"/>
-        <v>5.000000000000001E-2</v>
-      </c>
-      <c r="AA62" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="63" spans="2:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B63" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="C63" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="D63" s="8">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="62" spans="2:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B62" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="C62" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="D62" s="8">
         <v>100</v>
       </c>
-      <c r="E63" s="8"/>
-      <c r="F63" s="8"/>
-      <c r="G63" s="8"/>
-      <c r="H63" s="8"/>
-      <c r="I63" s="8"/>
-      <c r="J63" s="8"/>
-      <c r="K63" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="L63" s="8"/>
-      <c r="M63" s="8"/>
-      <c r="N63" s="8"/>
-      <c r="O63" s="8"/>
-      <c r="P63" s="8"/>
-      <c r="Q63" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="R63" s="8"/>
-      <c r="S63" s="8"/>
-      <c r="T63" s="8"/>
-      <c r="U63" s="8"/>
-      <c r="V63" s="8"/>
-      <c r="W63" s="8"/>
-      <c r="X63" s="8"/>
-      <c r="Y63" s="8"/>
-      <c r="Z63" s="19">
-        <f t="shared" si="5"/>
-        <v>100</v>
-      </c>
-      <c r="AA63" s="8" t="s">
-        <v>63</v>
+      <c r="E62" s="8"/>
+      <c r="F62" s="8"/>
+      <c r="G62" s="8"/>
+      <c r="H62" s="8"/>
+      <c r="I62" s="8"/>
+      <c r="J62" s="8"/>
+      <c r="K62" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="L62" s="8"/>
+      <c r="M62" s="8"/>
+      <c r="N62" s="8"/>
+      <c r="O62" s="8"/>
+      <c r="P62" s="8"/>
+      <c r="Q62" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="R62" s="8"/>
+      <c r="S62" s="8"/>
+      <c r="T62" s="8"/>
+      <c r="U62" s="8"/>
+      <c r="V62" s="8"/>
+      <c r="W62" s="8">
+        <v>-15</v>
+      </c>
+      <c r="X62" s="8"/>
+      <c r="Y62" s="8"/>
+      <c r="Z62" s="19">
+        <f>SUM(D62:J62,L62:P62,R62:Y62)</f>
+        <v>85</v>
+      </c>
+      <c r="AA62" s="8" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="80" spans="4:4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Add all stats for all guns
</commit_message>
<xml_diff>
--- a/Documentation/Balance/Balance.xlsx
+++ b/Documentation/Balance/Balance.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Tank-Survivors\Documentation\Balance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8EE1650-90C9-4019-946A-1044712B73D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA5391D7-32DC-4B09-A23C-44CBE6EE9162}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-16464" yWindow="6708" windowWidth="23040" windowHeight="13644" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-15240" yWindow="9360" windowWidth="23040" windowHeight="13644" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -367,7 +367,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFFFF00"/>
+      <color rgb="FF7030A0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -474,7 +474,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -503,10 +503,12 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -790,8 +792,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AG98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="J44" sqref="J44"/>
+    <sheetView tabSelected="1" topLeftCell="K17" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="Y50" sqref="Y50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1111,7 +1113,7 @@
       <c r="F7" s="11">
         <v>0.05</v>
       </c>
-      <c r="G7" s="30">
+      <c r="G7" s="28">
         <v>0.05</v>
       </c>
       <c r="H7" s="11">
@@ -2448,7 +2450,9 @@
       <c r="F35" s="1"/>
       <c r="G35" s="1"/>
       <c r="H35" s="1"/>
-      <c r="I35" s="1"/>
+      <c r="I35" s="1">
+        <v>20</v>
+      </c>
       <c r="J35" s="1">
         <v>20</v>
       </c>
@@ -2473,7 +2477,7 @@
       <c r="Y35" s="1"/>
       <c r="Z35" s="18">
         <f t="shared" si="3"/>
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="AA35" s="1" t="s">
         <v>6</v>
@@ -2627,11 +2631,11 @@
         <v>1</v>
       </c>
       <c r="E39" s="22"/>
-      <c r="F39" s="28">
+      <c r="F39" s="30">
         <v>0.5</v>
       </c>
       <c r="G39" s="22"/>
-      <c r="H39" s="28">
+      <c r="H39" s="30">
         <v>0.5</v>
       </c>
       <c r="I39" s="1"/>
@@ -2674,13 +2678,13 @@
         <v>20</v>
       </c>
       <c r="E40" s="22">
-        <v>5</v>
-      </c>
-      <c r="F40" s="1"/>
+        <v>10</v>
+      </c>
+      <c r="F40" s="30"/>
       <c r="G40" s="22">
-        <v>5</v>
-      </c>
-      <c r="H40" s="1"/>
+        <v>10</v>
+      </c>
+      <c r="H40" s="30"/>
       <c r="I40" s="1"/>
       <c r="J40" s="1"/>
       <c r="K40" s="1" t="s">
@@ -2704,7 +2708,7 @@
       <c r="Y40" s="1"/>
       <c r="Z40" s="18">
         <f t="shared" si="4"/>
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="AA40" s="1" t="s">
         <v>28</v>
@@ -2721,11 +2725,11 @@
         <v>10</v>
       </c>
       <c r="E41" s="1"/>
-      <c r="F41" s="1">
+      <c r="F41" s="30">
         <v>5</v>
       </c>
       <c r="G41" s="1"/>
-      <c r="H41" s="1">
+      <c r="H41" s="30">
         <v>5</v>
       </c>
       <c r="I41" s="1"/>
@@ -2777,15 +2781,15 @@
         <v>88</v>
       </c>
       <c r="L42" s="25">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="M42" s="25"/>
       <c r="N42" s="25">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="O42" s="25"/>
       <c r="P42" s="25">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="Q42" s="25" t="s">
         <v>88</v>
@@ -2800,7 +2804,7 @@
       <c r="Y42" s="25"/>
       <c r="Z42" s="27">
         <f t="shared" si="4"/>
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="AA42" s="25" t="s">
         <v>40</v>
@@ -2969,9 +2973,7 @@
       <c r="L46" s="25"/>
       <c r="M46" s="25"/>
       <c r="N46" s="25"/>
-      <c r="O46" s="25">
-        <v>-0.2</v>
-      </c>
+      <c r="O46" s="25"/>
       <c r="P46" s="25"/>
       <c r="Q46" s="25" t="s">
         <v>88</v>
@@ -2986,7 +2988,7 @@
       <c r="Y46" s="25"/>
       <c r="Z46" s="27">
         <f t="shared" si="4"/>
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
       <c r="AA46" s="25" t="s">
         <v>47</v>
@@ -3000,7 +3002,7 @@
         <v>48</v>
       </c>
       <c r="D47" s="26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E47" s="25"/>
       <c r="F47" s="25"/>
@@ -3019,25 +3021,25 @@
       <c r="Q47" s="25" t="s">
         <v>88</v>
       </c>
-      <c r="R47" s="22">
-        <v>1</v>
-      </c>
-      <c r="S47" s="25"/>
-      <c r="T47" s="22">
-        <v>1</v>
-      </c>
-      <c r="U47" s="25"/>
-      <c r="V47" s="22">
-        <v>1</v>
-      </c>
-      <c r="W47" s="25"/>
-      <c r="X47" s="22">
-        <v>1</v>
-      </c>
-      <c r="Y47" s="25"/>
+      <c r="R47" s="31">
+        <v>1</v>
+      </c>
+      <c r="S47" s="31"/>
+      <c r="T47" s="31">
+        <v>1</v>
+      </c>
+      <c r="U47" s="31"/>
+      <c r="V47" s="31">
+        <v>1</v>
+      </c>
+      <c r="W47" s="31"/>
+      <c r="X47" s="31">
+        <v>1</v>
+      </c>
+      <c r="Y47" s="31"/>
       <c r="Z47" s="27">
         <f t="shared" si="4"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AA47" s="25" t="s">
         <v>48</v>
@@ -3070,25 +3072,25 @@
       <c r="Q48" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="R48" s="22">
-        <v>5</v>
-      </c>
-      <c r="S48" s="1"/>
-      <c r="T48" s="22">
-        <v>5</v>
-      </c>
-      <c r="U48" s="1"/>
-      <c r="V48" s="22">
-        <v>5</v>
-      </c>
-      <c r="W48" s="1"/>
-      <c r="X48" s="22">
-        <v>5</v>
-      </c>
-      <c r="Y48" s="1"/>
+      <c r="R48" s="31">
+        <v>3</v>
+      </c>
+      <c r="S48" s="31"/>
+      <c r="T48" s="31">
+        <v>3</v>
+      </c>
+      <c r="U48" s="31"/>
+      <c r="V48" s="31">
+        <v>3</v>
+      </c>
+      <c r="W48" s="31"/>
+      <c r="X48" s="31">
+        <v>3</v>
+      </c>
+      <c r="Y48" s="31"/>
       <c r="Z48" s="18">
         <f t="shared" si="4"/>
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="AA48" s="1" t="s">
         <v>55</v>
@@ -3102,7 +3104,7 @@
         <v>56</v>
       </c>
       <c r="D49" s="13">
-        <v>0.1</v>
+        <v>0.7</v>
       </c>
       <c r="E49" s="1"/>
       <c r="F49" s="1"/>
@@ -3121,25 +3123,25 @@
       <c r="Q49" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="R49" s="22"/>
-      <c r="S49" s="1">
-        <v>-0.01</v>
-      </c>
-      <c r="T49" s="22"/>
-      <c r="U49" s="1">
-        <v>-0.01</v>
-      </c>
-      <c r="V49" s="22"/>
-      <c r="W49" s="1">
-        <v>-0.01</v>
-      </c>
-      <c r="X49" s="22"/>
-      <c r="Y49" s="1">
-        <v>-0.02</v>
+      <c r="R49" s="31"/>
+      <c r="S49" s="31">
+        <v>-0.1</v>
+      </c>
+      <c r="T49" s="31"/>
+      <c r="U49" s="31">
+        <v>-0.1</v>
+      </c>
+      <c r="V49" s="31"/>
+      <c r="W49" s="31">
+        <v>-0.1</v>
+      </c>
+      <c r="X49" s="31"/>
+      <c r="Y49" s="31">
+        <v>-0.1</v>
       </c>
       <c r="Z49" s="18">
         <f t="shared" si="4"/>
-        <v>5.0000000000000017E-2</v>
+        <v>0.30000000000000004</v>
       </c>
       <c r="AA49" s="1" t="s">
         <v>56</v>
@@ -3172,24 +3174,24 @@
       <c r="Q50" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="R50" s="29">
-        <v>1</v>
-      </c>
-      <c r="S50" s="8"/>
-      <c r="T50" s="29">
-        <v>1</v>
-      </c>
-      <c r="U50" s="8"/>
-      <c r="V50" s="29">
-        <v>1</v>
-      </c>
-      <c r="W50" s="8"/>
-      <c r="X50" s="29">
-        <v>1</v>
-      </c>
-      <c r="Y50" s="8"/>
+      <c r="R50" s="32"/>
+      <c r="S50" s="33">
+        <v>1</v>
+      </c>
+      <c r="T50" s="33"/>
+      <c r="U50" s="33">
+        <v>1</v>
+      </c>
+      <c r="V50" s="33"/>
+      <c r="W50" s="33">
+        <v>1</v>
+      </c>
+      <c r="X50" s="33"/>
+      <c r="Y50" s="33">
+        <v>1</v>
+      </c>
       <c r="Z50" s="18">
-        <f t="shared" si="4"/>
+        <f>SUM(D50:J50,L50:P50,S50:Y50)</f>
         <v>6</v>
       </c>
       <c r="AA50" s="8" t="s">
@@ -3391,7 +3393,7 @@
       <c r="X54" s="1"/>
       <c r="Y54" s="1"/>
       <c r="Z54" s="18">
-        <f t="shared" ref="Z54:Z63" si="5">SUM(D54:J54,L54:P54,R54:Y54)</f>
+        <f t="shared" ref="Z54:Z57" si="5">SUM(D54:J54,L54:P54,R54:Y54)</f>
         <v>4.6000000000000005</v>
       </c>
       <c r="AA54" s="1" t="s">
@@ -3846,7 +3848,7 @@
       <c r="AA84" s="14"/>
     </row>
     <row r="86" spans="2:27" x14ac:dyDescent="0.3">
-      <c r="C86" s="31"/>
+      <c r="C86" s="29"/>
     </row>
     <row r="91" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B91" s="15"/>

</xml_diff>